<commit_message>
Fixes after Testing phase 1
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>email</t>
   </si>
@@ -30,14 +30,39 @@
   </si>
   <si>
     <t>meet_date</t>
+  </si>
+  <si>
+    <t>kttinson.mec@gmail.com</t>
+  </si>
+  <si>
+    <t>KT TINSON MEC Subject</t>
+  </si>
+  <si>
+    <t>KT Tinson</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>tinsonkt3@gmail.com</t>
+  </si>
+  <si>
+    <t>Tinson 3 Subject</t>
+  </si>
+  <si>
+    <t>Tinson 3</t>
+  </si>
+  <si>
+    <t>Bravo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -119,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -134,6 +159,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -151,13 +180,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -191,7 +220,45 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>44512</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>43841</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="kttinson.mec@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="tinsonkt3@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>